<commit_message>
tutorial 1 is sone (for now)
Theres a few edits that angel should make at the end
</commit_message>
<xml_diff>
--- a/working_folder/LC3_grain_size_dist.xlsx
+++ b/working_folder/LC3_grain_size_dist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\MultiGrain\test_to_experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\MultiGrain\working_folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A584A5A-2B96-4A3F-A322-DEDE06A1B3FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FBA7C9-8F90-463C-B731-39B0F5DF1E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -367,7 +367,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -384,13 +384,13 @@
         <v>0</v>
       </c>
       <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>